<commit_message>
Klingon Ipsum > Lorem Ipsum
</commit_message>
<xml_diff>
--- a/data/cv_profile.xlsx
+++ b/data/cv_profile.xlsx
@@ -40,7 +40,7 @@
     <t xml:space="preserve">Profile</t>
   </si>
   <si>
-    <t xml:space="preserve">Lorem ipsum dolor sit amet, consectetur adipiscing elit. Pellentesque vitae sollicitudin orci, eget sagittis metus. Duis a varius dui. Nulla ac maximus neque. Pellentesque sollicitudin eros sed ligula blandit, facilisis tristique elit aliquam. Fusce rutrum aliquam suscipit. Pellentesque sollicitudin diam dolor, id congue nibh mattis id. Etiam in dapibus tellus, sed venenatis odio. Sed quis ipsum id quam bibendum accumsan in ac justo. Pellentesque quis nunc. </t>
+    <t xml:space="preserve">Bi'rel tlharghduj bor bur chadvay' lursa' ngop pin tlhoy' pipyus pujmoh qeylis qin vagh taq tey'be' yem 'orghen 'ud haqtaj. Boq dilyum dugh ghilasnos logh qewwi' qeylis quv bey' tangqa' verengan ha'dibah 'ab 'irnehnal. Be'joy' biqsip 'ugh boqha''egh butlh chang'eng cha'do' do'ha' jaghla' jornub marwi' matlh nguq pach per pop qevas qew qirq rura' pente' siv tagha' taq targh tiq tuy' tlhoy' sas 'ud'a'. Beb biqsip bo'degh choq dah ghojmeh taj ghuy'cha' ne' ngech pup qaj qaywi' qap raw' saqjan tagha' tey'.</t>
   </si>
 </sst>
 </file>
@@ -149,12 +149,12 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="76.57"/>

</xml_diff>

<commit_message>
Fixed profile text (too much text)
</commit_message>
<xml_diff>
--- a/data/cv_profile.xlsx
+++ b/data/cv_profile.xlsx
@@ -40,7 +40,7 @@
     <t xml:space="preserve">Profile</t>
   </si>
   <si>
-    <t xml:space="preserve">Bi'rel tlharghduj bor bur chadvay' lursa' ngop pin tlhoy' pipyus pujmoh qeylis qin vagh taq tey'be' yem 'orghen 'ud haqtaj. Boq dilyum dugh ghilasnos logh qewwi' qeylis quv bey' tangqa' verengan ha'dibah 'ab 'irnehnal. Be'joy' biqsip 'ugh boqha''egh butlh chang'eng cha'do' do'ha' jaghla' jornub marwi' matlh nguq pach per pop qevas qew qirq rura' pente' siv tagha' taq targh tiq tuy' tlhoy' sas 'ud'a'. Beb biqsip bo'degh choq dah ghojmeh taj ghuy'cha' ne' ngech pup qaj qaywi' qap raw' saqjan tagha' tey'.</t>
+    <t xml:space="preserve">Bi'rel tlharghduj bor bur chadvay' lursa' ngop pin tlhoy' pipyus pujmoh qeylis qin vagh taq tey'be' yem 'orghen 'ud haqtaj. Boq dilyum dugh ghilasnos logh qewwi' qeylis quv bey' tangqa' verengan ha'dibah 'ab 'irnehnal. Be'joy' biqsip 'ugh boqha''egh butlh chang'eng cha'do' do'ha' jaghla' jornub marwi' matlh nguq pach per pop qevas qew qirq rura' pente' siv tagha' taq targh tiq tuy' tlhoy' sas 'ud'a'.</t>
   </si>
 </sst>
 </file>
@@ -152,7 +152,7 @@
       <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.71"/>

</xml_diff>